<commit_message>
modify HLM model again and again, it can run.
</commit_message>
<xml_diff>
--- a/data/hlm/hlm_test_data.xlsx
+++ b/data/hlm/hlm_test_data.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D801B228-B04A-4E56-B2C8-E4FAFC794476}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="9264" yWindow="852" windowWidth="13068" windowHeight="11340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="erosion" sheetId="1" r:id="rId1"/>
@@ -15,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>埋存时间(年)</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -25,10 +26,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>北京</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>年均温度</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -54,13 +51,25 @@
   </si>
   <si>
     <t>站点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>敦煌 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>敦煌 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>敦煌 </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -117,7 +126,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -192,6 +201,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -227,6 +253,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -402,19 +445,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="30.5" customWidth="1"/>
+    <col min="2" max="2" width="30.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -422,7 +465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -430,18 +473,18 @@
         <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -452,62 +495,62 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>13</v>
+        <v>11.3</v>
       </c>
       <c r="C2">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="D2">
-        <v>488</v>
+        <v>48</v>
       </c>
       <c r="E2">
-        <v>59</v>
+        <v>7</v>
       </c>
       <c r="F2">
-        <v>1620</v>
+        <v>2632</v>
       </c>
       <c r="G2">
-        <v>4653</v>
+        <v>7846</v>
       </c>
       <c r="H2" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>